<commit_message>
New file 3D_Analysis_mat_file.py will pull data from *.mat file
</commit_message>
<xml_diff>
--- a/XH_Texture_Analysis/Features.xlsx
+++ b/XH_Texture_Analysis/Features.xlsx
@@ -518,7 +518,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>{'minimumROIDimensions': 2, 'minimumROISize': None, 'normalize': False, 'normalizeScale': 1, 'removeOutliers': None, 'resampledPixelSpacing': None, 'interpolator': 'sitkBSpline', 'preCrop': False, 'padDistance': 5, 'distances': [1], 'force2D': True, 'force2Ddimension': 0, 'resegmentRange': None, 'label': 1, 'additionalInfo': True}</t>
+          <t>{'minimumROIDimensions': 2, 'minimumROISize': None, 'normalize': False, 'normalizeScale': 1, 'removeOutliers': None, 'resampledPixelSpacing': None, 'interpolator': 'sitkBSpline', 'preCrop': False, 'padDistance': 5, 'distances': [1], 'force2D': True, 'force2Ddimension': 1, 'resegmentRange': None, 'label': 1, 'additionalInfo': True}</t>
         </is>
       </c>
     </row>
@@ -542,7 +542,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>05efd612eb295c36219aae36d5580db91ac7c76d</t>
+          <t>495af19c59d7d542db0ca5b8e8eb13e2bb6f11db</t>
         </is>
       </c>
     </row>
@@ -578,7 +578,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>(128, 128, 11)</t>
+          <t>(11, 128, 128)</t>
         </is>
       </c>
     </row>
@@ -589,7 +589,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.0005991712443338078</v>
+        <v>0.0005991712443338079</v>
       </c>
     </row>
     <row r="14">
@@ -620,7 +620,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>5a94293d4548feb386eea97c39f09503685f777f</t>
+          <t>6480027bb8478a1007f7ef316c31ecd33d347fc1</t>
         </is>
       </c>
     </row>
@@ -644,7 +644,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>(128, 128, 11)</t>
+          <t>(11, 128, 128)</t>
         </is>
       </c>
     </row>
@@ -656,7 +656,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>(14, 29, 2, 99, 77, 6)</t>
+          <t>(2, 14, 29, 6, 99, 77)</t>
         </is>
       </c>
     </row>
@@ -688,7 +688,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>(64.07568291050679, 68.0470280464805, 4.072519316176918)</t>
+          <t>(4.072519316176918, 64.07568291050679, 68.0470280464805)</t>
         </is>
       </c>
     </row>
@@ -700,7 +700,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>(64.07568291050679, 68.0470280464805, 4.072519316176918)</t>
+          <t>(4.072519316176918, 64.07568291050679, 68.0470280464805)</t>
         </is>
       </c>
     </row>
@@ -711,7 +711,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.6119074245935249</v>
+        <v>0.6119074245935252</v>
       </c>
     </row>
     <row r="25">
@@ -721,7 +721,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.05441635535643654</v>
+        <v>0.05441635535643636</v>
       </c>
     </row>
     <row r="26">
@@ -731,7 +731,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>6.212785569978326</v>
+        <v>6.212785569978303</v>
       </c>
     </row>
     <row r="27">
@@ -752,7 +752,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>99.0</t>
+          <t>75.02666192761077</t>
         </is>
       </c>
     </row>
@@ -764,7 +764,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>75.02666192761077</t>
+          <t>103.3537614216338</t>
         </is>
       </c>
     </row>
@@ -776,7 +776,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>103.3537614216338</t>
+          <t>99.0</t>
         </is>
       </c>
     </row>
@@ -800,7 +800,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>16358.458333333334</t>
+          <t>16331.125</t>
         </is>
       </c>
     </row>
@@ -811,7 +811,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>69.86226094665453</v>
+        <v>69.86226094665454</v>
       </c>
     </row>
     <row r="34">
@@ -822,7 +822,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>0.24498057532586015</t>
+          <t>0.24463083691313503</t>
         </is>
       </c>
     </row>
@@ -834,7 +834,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>12720.789195087067</t>
+          <t>12724.781255462323</t>
         </is>
       </c>
     </row>
@@ -846,7 +846,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>0.777627630665302</t>
+          <t>0.7791735875796875</t>
         </is>
       </c>
     </row>
@@ -892,7 +892,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>0.2648527424987449</t>
+          <t>0.26485274249874485</t>
         </is>
       </c>
     </row>
@@ -928,7 +928,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>3.5540948192351336</t>
+          <t>3.554094819235135</t>
         </is>
       </c>
     </row>
@@ -1012,7 +1012,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>0.0007023517575004792</t>
+          <t>0.000702351757500479</t>
         </is>
       </c>
     </row>
@@ -1024,7 +1024,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>0.004014125621856591</t>
+          <t>0.00401412562185659</t>
         </is>
       </c>
     </row>
@@ -1036,7 +1036,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>0.7343517640754207</t>
+          <t>0.734351764075421</t>
         </is>
       </c>
     </row>
@@ -1048,7 +1048,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>0.2648527424987449</t>
+          <t>0.26485274249874485</t>
         </is>
       </c>
     </row>
@@ -1372,7 +1372,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>1.0270836640777155</t>
+          <t>2.088274002939415</t>
         </is>
       </c>
     </row>
@@ -1384,7 +1384,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>11307.733832207823</t>
+          <t>5159.24262334976</t>
         </is>
       </c>
     </row>
@@ -1396,7 +1396,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>0.6879438968307978</t>
+          <t>0.3138798213390375</t>
         </is>
       </c>
     </row>
@@ -1408,7 +1408,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>1.1376179486116644</t>
+          <t>3.5133361151602465</t>
         </is>
       </c>
     </row>
@@ -1456,7 +1456,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>74.34902962827766</t>
+          <t>50.03790229360589</t>
         </is>
       </c>
     </row>
@@ -1468,7 +1468,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>74.34902962827766</t>
+          <t>50.03790229360589</t>
         </is>
       </c>
     </row>
@@ -1480,7 +1480,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>74.34902962827766</t>
+          <t>50.03790229360589</t>
         </is>
       </c>
     </row>
@@ -1504,7 +1504,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>0.01480371885696002</t>
+          <t>0.03125609187307063</t>
         </is>
       </c>
     </row>
@@ -1516,7 +1516,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>0.01480371885696002</t>
+          <t>0.03125609187307063</t>
         </is>
       </c>
     </row>
@@ -1528,7 +1528,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>0.01480371885696002</t>
+          <t>0.03125609187307063</t>
         </is>
       </c>
     </row>
@@ -1540,7 +1540,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>911.5</t>
+          <t>4477.25</t>
         </is>
       </c>
     </row>
@@ -1588,7 +1588,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>551.117736220648</t>
+          <t>294.20791718180163</t>
         </is>
       </c>
     </row>
@@ -1600,7 +1600,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>551.117736220648</t>
+          <t>294.20791718180163</t>
         </is>
       </c>
     </row>
@@ -1612,7 +1612,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>551.117736220648</t>
+          <t>294.20791718180163</t>
         </is>
       </c>
     </row>
@@ -1636,7 +1636,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>5.255708214301188</t>
+          <t>3.3127204580028766</t>
         </is>
       </c>
     </row>
@@ -1648,7 +1648,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>29.13658340328295</t>
+          <t>863.4486575512709</t>
         </is>
       </c>
     </row>
@@ -1660,7 +1660,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>0.030445702528915843</t>
+          <t>0.15369217280544734</t>
         </is>
       </c>
     </row>
@@ -1672,7 +1672,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>0.05545415830139319</t>
+          <t>0.2723885137190485</t>
         </is>
       </c>
     </row>
@@ -1684,7 +1684,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>151.29026876605664</t>
+          <t>88.7270692052786</t>
         </is>
       </c>
     </row>
@@ -1696,7 +1696,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>0.03646444886926772</t>
+          <t>0.2734596874304678</t>
         </is>
       </c>
     </row>
@@ -1708,7 +1708,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>0.03646444886926772</t>
+          <t>0.2734596874304678</t>
         </is>
       </c>
     </row>
@@ -1720,7 +1720,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>0.03646444886926772</t>
+          <t>0.2734596874304678</t>
         </is>
       </c>
     </row>
@@ -1732,7 +1732,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>12.0</t>
+          <t>106.0</t>
         </is>
       </c>
     </row>
@@ -1780,7 +1780,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>2049715.0833333333</t>
+          <t>35799.688679245286</t>
         </is>
       </c>
     </row>
@@ -1792,7 +1792,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>2049715.0833333333</t>
+          <t>35799.688679245286</t>
         </is>
       </c>
     </row>
@@ -1804,7 +1804,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>2049715.0833333333</t>
+          <t>35799.688679245286</t>
         </is>
       </c>
     </row>
@@ -1828,7 +1828,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>1.528301886792453</t>
         </is>
       </c>
     </row>
@@ -1840,7 +1840,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>0.08333333333333333</t>
+          <t>0.014417942328230687</t>
         </is>
       </c>
     </row>
@@ -1852,7 +1852,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>8.018606504418755e-07</t>
+          <t>0.019687902422080288</t>
         </is>
       </c>
     </row>
@@ -1864,7 +1864,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>8.018606504418755e-07</t>
+          <t>0.019687902422080288</t>
         </is>
       </c>
     </row>
@@ -1876,7 +1876,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>8.018606504418755e-07</t>
+          <t>0.019687902422080288</t>
         </is>
       </c>
     </row>
@@ -1888,7 +1888,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>3.5849625007211516</t>
+          <t>6.260847105465749</t>
         </is>
       </c>
     </row>
@@ -1900,7 +1900,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>0.0007300602299689724</t>
+          <t>0.006448865364725923</t>
         </is>
       </c>
     </row>
@@ -1912,7 +1912,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>173500.0208333333</t>
+          <t>11754.21262014952</t>
         </is>
       </c>
     </row>
@@ -2075,7 +2075,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>{'minimumROIDimensions': 2, 'minimumROISize': None, 'normalize': False, 'normalizeScale': 1, 'removeOutliers': None, 'resampledPixelSpacing': None, 'interpolator': 'sitkBSpline', 'preCrop': False, 'padDistance': 5, 'distances': [1], 'force2D': True, 'force2Ddimension': 0, 'resegmentRange': None, 'label': 1, 'additionalInfo': True}</t>
+          <t>{'minimumROIDimensions': 2, 'minimumROISize': None, 'normalize': False, 'normalizeScale': 1, 'removeOutliers': None, 'resampledPixelSpacing': None, 'interpolator': 'sitkBSpline', 'preCrop': False, 'padDistance': 5, 'distances': [1], 'force2D': True, 'force2Ddimension': 1, 'resegmentRange': None, 'label': 1, 'additionalInfo': True}</t>
         </is>
       </c>
     </row>
@@ -2099,7 +2099,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>56f3d77b755d51820745880a685ced9743aeccae</t>
+          <t>46a358991d378c72b3885f729d4b38f3cab8cd27</t>
         </is>
       </c>
     </row>
@@ -2135,7 +2135,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>(112, 112, 20)</t>
+          <t>(20, 112, 112)</t>
         </is>
       </c>
     </row>
@@ -2177,7 +2177,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>b68ea80f6a8b4e7d39eca3914535929e7b8c8e48</t>
+          <t>0f17e74835fa80fbfec56204e472e595de0040ce</t>
         </is>
       </c>
     </row>
@@ -2201,7 +2201,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>(112, 112, 20)</t>
+          <t>(20, 112, 112)</t>
         </is>
       </c>
     </row>
@@ -2213,7 +2213,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>(11, 26, 3, 90, 67, 13)</t>
+          <t>(3, 11, 26, 13, 90, 67)</t>
         </is>
       </c>
     </row>
@@ -2245,7 +2245,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>(53.26389535622063, 64.07111713160903, 9.679295601744062)</t>
+          <t>(9.679295601744062, 53.26389535622063, 64.07111713160903)</t>
         </is>
       </c>
     </row>
@@ -2257,7 +2257,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>(53.26389535622063, 64.07111713160903, 9.679295601744062)</t>
+          <t>(9.679295601744062, 53.26389535622063, 64.07111713160903)</t>
         </is>
       </c>
     </row>
@@ -2268,7 +2268,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.5870883708257714</v>
+        <v>0.5870883708257715</v>
       </c>
     </row>
     <row r="25">
@@ -2278,7 +2278,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.1179501609873498</v>
+        <v>0.1179501609873502</v>
       </c>
     </row>
     <row r="26">
@@ -2288,7 +2288,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>12.26882798837458</v>
+        <v>12.26882798837461</v>
       </c>
     </row>
     <row r="27">
@@ -2309,7 +2309,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>90.0</t>
+          <t>64.19501538281614</t>
         </is>
       </c>
     </row>
@@ -2321,7 +2321,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>64.19501538281614</t>
+          <t>90.52071586106685</t>
         </is>
       </c>
     </row>
@@ -2333,7 +2333,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>90.52071586106685</t>
+          <t>90.0</t>
         </is>
       </c>
     </row>
@@ -2357,7 +2357,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>23495.416666666668</t>
+          <t>23576.916666666668</t>
         </is>
       </c>
     </row>
@@ -2379,7 +2379,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>0.32191335577134633</t>
+          <t>0.3227027086284717</t>
         </is>
       </c>
     </row>
@@ -2391,7 +2391,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>12323.495095080543</t>
+          <t>12321.763044272322</t>
         </is>
       </c>
     </row>
@@ -2403,7 +2403,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>0.5245063439357552</t>
+          <t>0.5226197818179076</t>
         </is>
       </c>
     </row>
@@ -2569,7 +2569,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>28.25924645039548</t>
+          <t>28.259246450395477</t>
         </is>
       </c>
     </row>
@@ -2641,7 +2641,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>82.02092533893554</t>
+          <t>81.78231654291814</t>
         </is>
       </c>
     </row>
@@ -2653,7 +2653,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>464.2482785331009</t>
+          <t>329.13983487908786</t>
         </is>
       </c>
     </row>
@@ -2665,7 +2665,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>8.79123372253927</t>
+          <t>4.8829421383276355</t>
         </is>
       </c>
     </row>
@@ -2677,7 +2677,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>12.820520985060543</t>
+          <t>10.893700373687226</t>
         </is>
       </c>
     </row>
@@ -2689,7 +2689,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>1.849757229768806</t>
+          <t>2.955136082816319</t>
         </is>
       </c>
     </row>
@@ -2701,7 +2701,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>0.7475076108066054</t>
+          <t>0.5683232899377325</t>
         </is>
       </c>
     </row>
@@ -2713,7 +2713,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>0.9923709075973743</t>
+          <t>1.2784226342795266</t>
         </is>
       </c>
     </row>
@@ -2725,7 +2725,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>1.7908663399873557</t>
+          <t>2.035933787977756</t>
         </is>
       </c>
     </row>
@@ -2737,7 +2737,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>0.8563806334045001</t>
+          <t>1.2681842586068017</t>
         </is>
       </c>
     </row>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>0.616801493943455</t>
+          <t>0.5589200856216024</t>
         </is>
       </c>
     </row>
@@ -2761,7 +2761,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>0.585065815200138</t>
+          <t>0.5121995782326997</t>
         </is>
       </c>
     </row>
@@ -2773,7 +2773,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>0.9937561430205955</t>
+          <t>0.9901672473612</t>
         </is>
       </c>
     </row>
@@ -2785,7 +2785,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>0.9472492215225297</t>
+          <t>0.9335101904356978</t>
         </is>
       </c>
     </row>
@@ -2797,7 +2797,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>-0.2073678239136259</t>
+          <t>-0.11803646506185317</t>
         </is>
       </c>
     </row>
@@ -2809,7 +2809,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>0.8372200619140349</t>
+          <t>0.6645998614360357</t>
         </is>
       </c>
     </row>
@@ -2821,7 +2821,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>0.4934351226128816</t>
+          <t>0.46654884606650054</t>
         </is>
       </c>
     </row>
@@ -2833,7 +2833,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>8.903831601602063</t>
+          <t>8.932930109560195</t>
         </is>
       </c>
     </row>
@@ -2845,7 +2845,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>0.03387563319849619</t>
+          <t>0.02964035254761465</t>
         </is>
       </c>
     </row>
@@ -2857,7 +2857,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>5.3313478833066625</t>
+          <t>5.521256156953849</t>
         </is>
       </c>
     </row>
@@ -2869,7 +2869,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>0.7552311442112154</t>
+          <t>0.5810208453185983</t>
         </is>
       </c>
     </row>
@@ -2881,7 +2881,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>0.06459595948501753</t>
+          <t>0.05561546315487343</t>
         </is>
       </c>
     </row>
@@ -2893,7 +2893,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>17.807663203204136</t>
+          <t>17.865860219120393</t>
         </is>
       </c>
     </row>
@@ -2905,7 +2905,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>3.8680636975191343</t>
+          <t>3.7505544294864235</t>
         </is>
       </c>
     </row>
@@ -2917,7 +2917,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>3.667569553707337</t>
+          <t>3.462209114125886</t>
         </is>
       </c>
     </row>
@@ -2929,7 +2929,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>5.621073709805425</t>
+          <t>5.3328199487154215</t>
         </is>
       </c>
     </row>
@@ -2941,7 +2941,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>4130.989755746518</t>
+          <t>5018.567624772468</t>
         </is>
       </c>
     </row>
@@ -2953,7 +2953,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>0.1748715131755712</t>
+          <t>0.2124441275355572</t>
         </is>
       </c>
     </row>
@@ -2965,7 +2965,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>2.5908792676169607</t>
+          <t>1.9031747499139091</t>
         </is>
       </c>
     </row>
@@ -3013,7 +3013,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>14.065487025356644</t>
+          <t>9.434915125089955</t>
         </is>
       </c>
     </row>
@@ -3025,7 +3025,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>1135.2299030605766</t>
+          <t>766.5860390297591</t>
         </is>
       </c>
     </row>
@@ -3037,7 +3037,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>0.20668452076460553</t>
+          <t>0.13477769550242</t>
         </is>
       </c>
     </row>
@@ -3061,7 +3061,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>0.21968244983182378</t>
+          <t>0.31289156617358377</t>
         </is>
       </c>
     </row>
@@ -3073,7 +3073,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>18.120591070259227</t>
+          <t>25.847289856120415</t>
         </is>
       </c>
     </row>
@@ -3085,7 +3085,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>0.003665291601199343</t>
+          <t>0.005180856549480977</t>
         </is>
       </c>
     </row>
@@ -3097,7 +3097,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>2274.0672722944755</t>
+          <t>2519.2851768817522</t>
         </is>
       </c>
     </row>
@@ -3109,7 +3109,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>0.13721456264587506</t>
+          <t>0.1364085778489954</t>
         </is>
       </c>
     </row>
@@ -3121,7 +3121,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>4.0925448307453</t>
+          <t>4.122034497702346</t>
         </is>
       </c>
     </row>
@@ -3133,7 +3133,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>82.83653563364774</t>
+          <t>82.648096659989</t>
         </is>
       </c>
     </row>
@@ -3145,7 +3145,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>2.737586388806821</t>
+          <t>2.1043879175831446</t>
         </is>
       </c>
     </row>
@@ -3157,7 +3157,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>222.8234908952357</t>
+          <t>172.32345237200164</t>
         </is>
       </c>
     </row>
@@ -3169,7 +3169,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>0.04081284693535755</t>
+          <t>0.031114582533886256</t>
         </is>
       </c>
     </row>
@@ -3181,7 +3181,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>0.015281343171409294</t>
+          <t>0.015306860081176921</t>
         </is>
       </c>
     </row>
@@ -3193,7 +3193,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>4.2928780999723</t>
+          <t>4.00453949988683</t>
         </is>
       </c>
     </row>
@@ -3205,7 +3205,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>9199.031285950352</t>
+          <t>12216.407308076783</t>
         </is>
       </c>
     </row>
@@ -3217,7 +3217,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>0.5535804569734117</t>
+          <t>0.6541900739721184</t>
         </is>
       </c>
     </row>
@@ -3229,7 +3229,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>0.7015726199043305</t>
+          <t>0.7819497946916141</t>
         </is>
       </c>
     </row>
@@ -3241,7 +3241,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>0.6954283218582642</t>
+          <t>0.42645213959203965</t>
         </is>
       </c>
     </row>
@@ -3253,7 +3253,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>0.7713553758905922</t>
+          <t>0.8332849364240101</t>
         </is>
       </c>
     </row>
@@ -3265,7 +3265,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>64.03741913703878</t>
+          <t>68.98875592485689</t>
         </is>
       </c>
     </row>
@@ -3277,7 +3277,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>0.01195521920356139</t>
+          <t>0.012924390447750785</t>
         </is>
       </c>
     </row>
@@ -3289,7 +3289,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>704.8059928897918</t>
+          <t>1065.8516056338028</t>
         </is>
       </c>
     </row>
@@ -3301,7 +3301,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>0.11931708022512134</t>
+          <t>0.12009595556437215</t>
         </is>
       </c>
     </row>
@@ -3313,7 +3313,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>5.291718149573567</t>
+          <t>5.207420952985519</t>
         </is>
       </c>
     </row>
@@ -3325,7 +3325,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>83.06399187404774</t>
+          <t>83.23752112676057</t>
         </is>
       </c>
     </row>
@@ -3337,7 +3337,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>93.22312510580667</t>
+          <t>19.50794366197183</t>
         </is>
       </c>
     </row>
@@ -3349,7 +3349,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>6809.5046554934825</t>
+          <t>1561.046985915493</t>
         </is>
       </c>
     </row>
@@ -3361,7 +3361,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>1.5128718931566205</t>
+          <t>0.2776125421365203</t>
         </is>
       </c>
     </row>
@@ -3373,7 +3373,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>0.016661711204767667</t>
+          <t>0.01629321570319979</t>
         </is>
       </c>
     </row>
@@ -3385,7 +3385,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>1695.126968004063</t>
+          <t>2955.1302535211266</t>
         </is>
       </c>
     </row>
@@ -3397,7 +3397,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>0.28696918368106705</t>
+          <t>0.33297242293195795</t>
         </is>
       </c>
     </row>
@@ -3409,7 +3409,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>0.5522024742621118</t>
+          <t>0.5964133455997646</t>
         </is>
       </c>
     </row>
@@ -3421,7 +3421,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>45.22637356620855</t>
+          <t>49.19127953228129</t>
         </is>
       </c>
     </row>
@@ -3433,7 +3433,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>0.009876633623061152</t>
+          <t>0.010356307620190307</t>
         </is>
       </c>
     </row>
@@ -3445,7 +3445,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>5.915623935324845</t>
+          <t>5.51061627520538</t>
         </is>
       </c>
     </row>
@@ -3457,7 +3457,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>0.2500529145324472</t>
+          <t>0.3756931803750582</t>
         </is>
       </c>
     </row>
@@ -3469,7 +3469,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>77.22989601620675</t>
+          <t>12.423049344177741</t>
         </is>
       </c>
     </row>
@@ -3481,7 +3481,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>11.846509393594468</t>
+          <t>15.161771462749808</t>
         </is>
       </c>
     </row>
@@ -3493,7 +3493,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>0.00044465309708067313</t>
+          <t>0.0003474255699209513</t>
         </is>
       </c>
     </row>
@@ -3505,7 +3505,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>94.66630168775043</t>
+          <t>125.00159906914004</t>
         </is>
       </c>
     </row>
@@ -3517,7 +3517,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>0.020627197313893</t>
+          <t>0.027331259582437945</t>
         </is>
       </c>
     </row>
@@ -3529,7 +3529,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>0.05488351407263045</t>
+          <t>0.041421181875694185</t>
         </is>
       </c>
     </row>
@@ -3632,7 +3632,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>{'minimumROIDimensions': 2, 'minimumROISize': None, 'normalize': False, 'normalizeScale': 1, 'removeOutliers': None, 'resampledPixelSpacing': None, 'interpolator': 'sitkBSpline', 'preCrop': False, 'padDistance': 5, 'distances': [1], 'force2D': True, 'force2Ddimension': 0, 'resegmentRange': None, 'label': 1, 'additionalInfo': True}</t>
+          <t>{'minimumROIDimensions': 2, 'minimumROISize': None, 'normalize': False, 'normalizeScale': 1, 'removeOutliers': None, 'resampledPixelSpacing': None, 'interpolator': 'sitkBSpline', 'preCrop': False, 'padDistance': 5, 'distances': [1], 'force2D': True, 'force2Ddimension': 1, 'resegmentRange': None, 'label': 1, 'additionalInfo': True}</t>
         </is>
       </c>
     </row>
@@ -3656,7 +3656,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>c5aa124cc311af0bcef4559f6b36ae7f5d1e9333</t>
+          <t>9e7a19a89ff9e2297589ef61f39ba7ad80ebc747</t>
         </is>
       </c>
     </row>
@@ -3692,7 +3692,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>(112, 112, 8)</t>
+          <t>(8, 112, 112)</t>
         </is>
       </c>
     </row>
@@ -3703,7 +3703,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1092.508808992347</v>
+        <v>979.3355728363504</v>
       </c>
     </row>
     <row r="14">
@@ -3734,7 +3734,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>488bdc033de9002e7e0ceb8afc33117efc97d674</t>
+          <t>544e9de332749d352474c9faaf5baf9cf2b0a162</t>
         </is>
       </c>
     </row>
@@ -3758,7 +3758,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>(112, 112, 8)</t>
+          <t>(8, 112, 112)</t>
         </is>
       </c>
     </row>
@@ -3770,7 +3770,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>(5, 21, 0, 104, 71, 8)</t>
+          <t>(0, 5, 21, 8, 104, 71)</t>
         </is>
       </c>
     </row>
@@ -3802,7 +3802,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>(54.580562153602536, 58.84976247030879, 2.8822743467933494)</t>
+          <t>(2.8822743467933494, 54.580562153602536, 58.84976247030879)</t>
         </is>
       </c>
     </row>
@@ -3814,7 +3814,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>(54.580562153602536, 58.84976247030879, 2.8822743467933494)</t>
+          <t>(2.8822743467933494, 54.580562153602536, 58.84976247030879)</t>
         </is>
       </c>
     </row>
@@ -3835,7 +3835,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.06636270622148056</v>
+        <v>0.06636270622148019</v>
       </c>
     </row>
     <row r="26">
@@ -3845,7 +3845,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>8.029749984761613</v>
+        <v>8.029749984761569</v>
       </c>
     </row>
     <row r="27">
@@ -3855,7 +3855,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>120.9979285347847</v>
+        <v>120.9979285347846</v>
       </c>
     </row>
     <row r="28">
@@ -3866,7 +3866,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>104.00480758118829</t>
+          <t>70.00714249274856</t>
         </is>
       </c>
     </row>
@@ -3878,7 +3878,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>70.00714249274856</t>
+          <t>105.11898020814318</t>
         </is>
       </c>
     </row>
@@ -3890,7 +3890,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>105.11898020814318</t>
+          <t>104.00480758118829</t>
         </is>
       </c>
     </row>
@@ -3914,7 +3914,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>20250.5</t>
+          <t>20519.916666666668</t>
         </is>
       </c>
     </row>
@@ -3925,7 +3925,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>62.94515879244346</v>
+        <v>62.94515879244344</v>
       </c>
     </row>
     <row r="34">
@@ -3936,7 +3936,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>0.1831885841485933</t>
+          <t>0.18470999584251063</t>
         </is>
       </c>
     </row>
@@ -3948,7 +3948,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>19612.948393988787</t>
+          <t>19623.544496815608</t>
         </is>
       </c>
     </row>
@@ -3960,7 +3960,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>0.9685167474377812</t>
+          <t>0.9563169683185332</t>
         </is>
       </c>
     </row>
@@ -3982,7 +3982,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>1714.0</t>
+          <t>1798.773828125</t>
         </is>
       </c>
     </row>
@@ -3994,7 +3994,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>6172.0</t>
+          <t>4983.680175781249</t>
         </is>
       </c>
     </row>
@@ -4006,7 +4006,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>343095718506.0</t>
+          <t>246501949270.9411</t>
         </is>
       </c>
     </row>
@@ -4018,7 +4018,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>8.003248866941965</t>
+          <t>7.640876906694744</t>
         </is>
       </c>
     </row>
@@ -4030,7 +4030,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>2400.0</t>
+          <t>1764.220703125</t>
         </is>
       </c>
     </row>
@@ -4042,7 +4042,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>3.254985558207785</t>
+          <t>2.957836844446989</t>
         </is>
       </c>
     </row>
@@ -4054,7 +4054,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>11553.0</t>
+          <t>8943.5361328125</t>
         </is>
       </c>
     </row>
@@ -4066,7 +4066,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>1406.8829190179065</t>
+          <t>1016.413486370395</t>
         </is>
       </c>
     </row>
@@ -4078,7 +4078,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>3730.9636777513856</t>
+          <t>3259.4342120752767</t>
         </is>
       </c>
     </row>
@@ -4090,7 +4090,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>3459.0</t>
+          <t>3126.970703125</t>
         </is>
       </c>
     </row>
@@ -4114,7 +4114,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>11553.0</t>
+          <t>8943.5361328125</t>
         </is>
       </c>
     </row>
@@ -4126,7 +4126,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>1000.152971827943</t>
+          <t>728.7578348001308</t>
         </is>
       </c>
     </row>
@@ -4138,7 +4138,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>4120.462657899295</t>
+          <t>3492.59728727941</t>
         </is>
       </c>
     </row>
@@ -4150,7 +4150,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>0.696800197940182</t>
+          <t>0.4059001796420181</t>
         </is>
       </c>
     </row>
@@ -4162,7 +4162,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>343095718506.0</t>
+          <t>246501949270.9411</t>
         </is>
       </c>
     </row>
@@ -4174,7 +4174,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>0.004692444617153417</t>
+          <t>0.005801849012549766</t>
         </is>
       </c>
     </row>
@@ -4186,7 +4186,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>3058122.550442373</t>
+          <t>1574324.428264717</t>
         </is>
       </c>
     </row>
@@ -4198,7 +4198,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>26908.49525868749</t>
+          <t>18373.29553894354</t>
         </is>
       </c>
     </row>
@@ -4210,7 +4210,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>798655640.3521831</t>
+          <t>100705310.94835672</t>
         </is>
       </c>
     </row>
@@ -4222,7 +4222,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>1324099.135520839</t>
+          <t>134549.0269677298</t>
         </is>
       </c>
     </row>
@@ -4234,7 +4234,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>15737.735354990167</t>
+          <t>5745.125838052084</t>
         </is>
       </c>
     </row>
@@ -4246,7 +4246,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>2997.670690721592</t>
+          <t>3924.7746401431727</t>
         </is>
       </c>
     </row>
@@ -4258,7 +4258,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>0.6799408836349686</t>
+          <t>0.1913228465342073</t>
         </is>
       </c>
     </row>
@@ -4270,7 +4270,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>41.66821324751565</t>
+          <t>48.64134868240853</t>
         </is>
       </c>
     </row>
@@ -4282,7 +4282,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>6.7829958563628585</t>
+          <t>6.953395178854253</t>
         </is>
       </c>
     </row>
@@ -4294,7 +4294,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>1236.8161735018928</t>
+          <t>1471.303966850348</t>
         </is>
       </c>
     </row>
@@ -4306,7 +4306,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>0.06861933086985078</t>
+          <t>0.059577293121687594</t>
         </is>
       </c>
     </row>
@@ -4318,7 +4318,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>0.027710524576336076</t>
+          <t>0.022852020066269192</t>
         </is>
       </c>
     </row>
@@ -4330,7 +4330,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>0.986731858588465</t>
+          <t>0.9721070249742207</t>
         </is>
       </c>
     </row>
@@ -4342,7 +4342,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>0.9216156734426916</t>
+          <t>0.888005944964247</t>
         </is>
       </c>
     </row>
@@ -4354,7 +4354,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>-0.21561195802724722</t>
+          <t>-0.1729093999223375</t>
         </is>
       </c>
     </row>
@@ -4366,7 +4366,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>0.9838047679711038</t>
+          <t>0.9632069991032123</t>
         </is>
       </c>
     </row>
@@ -4378,7 +4378,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>0.027589375145288333</t>
+          <t>0.023502136529601692</t>
         </is>
       </c>
     </row>
@@ -4390,7 +4390,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>154.02322085103512</t>
+          <t>133.85885086522626</t>
         </is>
       </c>
     </row>
@@ -4402,7 +4402,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>6.191042449145834e-05</t>
+          <t>7.553816661144654e-05</t>
         </is>
       </c>
     </row>
@@ -4414,7 +4414,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>14.238990620654473</t>
+          <t>13.905722241923158</t>
         </is>
       </c>
     </row>
@@ -4426,7 +4426,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>0.73034894701696</t>
+          <t>0.43908890631191266</t>
         </is>
       </c>
     </row>
@@ -4438,7 +4438,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>0.00029775480819921806</t>
+          <t>0.000311527342502993</t>
         </is>
       </c>
     </row>
@@ -4450,7 +4450,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>308.0464417020685</t>
+          <t>267.717701730452</t>
         </is>
       </c>
     </row>
@@ -4462,7 +4462,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>8.900946986473725</t>
+          <t>8.2319071428868</t>
         </is>
       </c>
     </row>
@@ -4474,7 +4474,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>4683.851511427951</t>
+          <t>2417.4751195488143</t>
         </is>
       </c>
     </row>
@@ -4486,7 +4486,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>8.335353678395913</t>
+          <t>7.875430199132992</t>
         </is>
       </c>
     </row>
@@ -4498,7 +4498,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>17714.106789390342</t>
+          <t>18572.44368566904</t>
         </is>
       </c>
     </row>
@@ -4510,7 +4510,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>0.8765888157853494</t>
+          <t>0.9190639195204395</t>
         </is>
       </c>
     </row>
@@ -4522,7 +4522,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>0.07153415249418714</t>
+          <t>0.04316964221345825</t>
         </is>
       </c>
     </row>
@@ -4534,7 +4534,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>94.82492082343626</t>
+          <t>117.2437648456057</t>
         </is>
       </c>
     </row>
@@ -4546,7 +4546,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>4892.909581670892</t>
+          <t>2518.6597323480105</t>
         </is>
       </c>
     </row>
@@ -4558,7 +4558,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>27320.254552652415</t>
+          <t>19647.585956057006</t>
         </is>
       </c>
     </row>
@@ -4570,7 +4570,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>1.2144695170229611</t>
+          <t>1.1313341250989708</t>
         </is>
       </c>
     </row>
@@ -4582,7 +4582,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>32146.309679334918</t>
+          <t>21854.233422406967</t>
         </is>
       </c>
     </row>
@@ -4594,7 +4594,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>0.003272792828672127</t>
+          <t>0.0028827908009235598</t>
         </is>
       </c>
     </row>
@@ -4606,7 +4606,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>0.0015710238401406454</t>
+          <t>0.0015837986211828426</t>
         </is>
       </c>
     </row>
@@ -4618,7 +4618,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>0.9501902436878684</t>
+          <t>0.9682111594967888</t>
         </is>
       </c>
     </row>
@@ -4630,7 +4630,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>26177.47084969099</t>
+          <t>19113.14345253805</t>
         </is>
       </c>
     </row>
@@ -4642,7 +4642,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>0.001255869132357564</t>
+          <t>0.0013141457374811977</t>
         </is>
       </c>
     </row>
@@ -4654,7 +4654,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>93.76782438639805</t>
+          <t>116.49066698212361</t>
         </is>
       </c>
     </row>
@@ -4666,7 +4666,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>0.004680550846285107</t>
+          <t>0.005795841138313658</t>
         </is>
       </c>
     </row>
@@ -4678,7 +4678,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>4902.517207818948</t>
+          <t>2521.598938059845</t>
         </is>
       </c>
     </row>
@@ -4690,7 +4690,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>27360.554039221737</t>
+          <t>19663.014326848403</t>
         </is>
       </c>
     </row>
@@ -4702,7 +4702,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>1.026311926624756</t>
+          <t>1.0164130696211242</t>
         </is>
       </c>
     </row>
@@ -4714,7 +4714,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>27955.853571000196</t>
+          <t>19938.546016669596</t>
         </is>
       </c>
     </row>
@@ -4726,7 +4726,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>0.0017361325805070643</t>
+          <t>0.0017183461996920085</t>
         </is>
       </c>
     </row>
@@ -4738,7 +4738,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>0.0015214994769496193</t>
+          <t>0.001541919606620412</t>
         </is>
       </c>
     </row>
@@ -4750,7 +4750,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>8.067556798114168</t>
+          <t>7.682704503899393</t>
         </is>
       </c>
     </row>
@@ -4762,7 +4762,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>19691.017773174688</t>
+          <t>19884.862764107173</t>
         </is>
       </c>
     </row>
@@ -4774,7 +4774,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>0.9829008817414707</t>
+          <t>0.9893341089865824</t>
         </is>
       </c>
     </row>
@@ -4786,7 +4786,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>0.9913648060174189</t>
+          <t>0.9946060965954078</t>
         </is>
       </c>
     </row>
@@ -4798,7 +4798,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>0.008809368087062633</t>
+          <t>0.005518544774245316</t>
         </is>
       </c>
     </row>
@@ -4810,7 +4810,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>0.993519174035695</t>
+          <t>0.9959661319295958</t>
         </is>
       </c>
     </row>
@@ -4822,7 +4822,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>27212.910951359176</t>
+          <t>19595.128048241266</t>
         </is>
       </c>
     </row>
@@ -4834,7 +4834,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>0.0014817290293999944</t>
+          <t>0.0015116976242283966</t>
         </is>
       </c>
     </row>
@@ -4846,7 +4846,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>90.7073495518566</t>
+          <t>114.24585355987055</t>
         </is>
       </c>
     </row>
@@ -4858,7 +4858,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>0.004645702921990094</t>
+          <t>0.005776995022242645</t>
         </is>
       </c>
     </row>
@@ -4870,7 +4870,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>4930.0624154422985</t>
+          <t>2530.7584800493687</t>
         </is>
       </c>
     </row>
@@ -4882,7 +4882,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>27477.28819462228</t>
+          <t>19710.046116504855</t>
         </is>
       </c>
     </row>
@@ -4894,7 +4894,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>1.1089372599231755</t>
+          <t>1.0666464401294498</t>
         </is>
       </c>
     </row>
@@ -4906,7 +4906,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>29940.76947503201</t>
+          <t>20826.741454288025</t>
         </is>
       </c>
     </row>
@@ -4918,7 +4918,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>0.0023496334902727727</t>
+          <t>0.002128265680566545</t>
         </is>
       </c>
     </row>
@@ -4930,7 +4930,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>0.0013667461658771584</t>
+          <t>0.001414081901195987</t>
         </is>
       </c>
     </row>
@@ -4942,7 +4942,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>18270.041638924456</t>
+          <t>18951.46875</t>
         </is>
       </c>
     </row>
@@ -4954,7 +4954,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>0.935725564093442</t>
+          <t>0.9583064699635923</t>
         </is>
       </c>
     </row>
@@ -4966,7 +4966,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>0.9748783610755442</t>
+          <t>0.9839564230492629</t>
         </is>
       </c>
     </row>
@@ -4978,7 +4978,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>26896.632238227343</t>
+          <t>19440.034116830724</t>
         </is>
       </c>
     </row>
@@ -4990,7 +4990,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>0.0012350097517870797</t>
+          <t>0.0012917809515326619</t>
         </is>
       </c>
     </row>
@@ -5002,7 +5002,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>8.214512119485223</t>
+          <t>7.785584249652091</t>
         </is>
       </c>
     </row>
@@ -5014,7 +5014,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>0.966201504354711</t>
+          <t>0.9786223277909739</t>
         </is>
       </c>
     </row>
@@ -5026,7 +5026,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>0.03775201627645046</t>
+          <t>0.02247993056210136</t>
         </is>
       </c>
     </row>
@@ -5038,7 +5038,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>0.03749026844251277</t>
+          <t>0.08756014363803473</t>
         </is>
       </c>
     </row>
@@ -5050,7 +5050,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>0.00045621281903517464</t>
+          <t>0.00028743674103002745</t>
         </is>
       </c>
     </row>
@@ -5062,7 +5062,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>1944389.280764767</t>
+          <t>1432040.2202054507</t>
         </is>
       </c>
     </row>
@@ -5074,7 +5074,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>1.5598974985021423</t>
+          <t>1.8315213024437824</t>
         </is>
       </c>
     </row>
@@ -5086,7 +5086,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>34.65100230304412</t>
+          <t>10.181439206275076</t>
         </is>
       </c>
     </row>
@@ -5128,7 +5128,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.6119074245935249</v>
+        <v>0.6119074245935252</v>
       </c>
     </row>
     <row r="3">
@@ -5138,7 +5138,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.05441635535643654</v>
+        <v>0.05441635535643636</v>
       </c>
     </row>
     <row r="4">
@@ -5148,7 +5148,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6.212785569978326</v>
+        <v>6.212785569978303</v>
       </c>
     </row>
     <row r="5">
@@ -5169,7 +5169,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>99.0</t>
+          <t>75.02666192761077</t>
         </is>
       </c>
     </row>
@@ -5181,7 +5181,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>75.02666192761077</t>
+          <t>103.3537614216338</t>
         </is>
       </c>
     </row>
@@ -5193,7 +5193,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>103.3537614216338</t>
+          <t>99.0</t>
         </is>
       </c>
     </row>
@@ -5217,7 +5217,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>16358.458333333334</t>
+          <t>16331.125</t>
         </is>
       </c>
     </row>
@@ -5228,7 +5228,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>69.86226094665453</v>
+        <v>69.86226094665454</v>
       </c>
     </row>
     <row r="12">
@@ -5239,7 +5239,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>0.24498057532586015</t>
+          <t>0.24463083691313503</t>
         </is>
       </c>
     </row>
@@ -5251,7 +5251,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>12720.789195087067</t>
+          <t>12724.781255462323</t>
         </is>
       </c>
     </row>
@@ -5263,7 +5263,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>0.777627630665302</t>
+          <t>0.7791735875796875</t>
         </is>
       </c>
     </row>
@@ -5309,7 +5309,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>0.2648527424987449</t>
+          <t>0.26485274249874485</t>
         </is>
       </c>
     </row>
@@ -5345,7 +5345,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>3.5540948192351336</t>
+          <t>3.554094819235135</t>
         </is>
       </c>
     </row>
@@ -5429,7 +5429,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>0.0007023517575004792</t>
+          <t>0.000702351757500479</t>
         </is>
       </c>
     </row>
@@ -5441,7 +5441,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>0.004014125621856591</t>
+          <t>0.00401412562185659</t>
         </is>
       </c>
     </row>
@@ -5453,7 +5453,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>0.7343517640754207</t>
+          <t>0.734351764075421</t>
         </is>
       </c>
     </row>
@@ -5465,7 +5465,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>0.2648527424987449</t>
+          <t>0.26485274249874485</t>
         </is>
       </c>
     </row>
@@ -5789,7 +5789,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>1.0270836640777155</t>
+          <t>2.088274002939415</t>
         </is>
       </c>
     </row>
@@ -5801,7 +5801,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>11307.733832207823</t>
+          <t>5159.24262334976</t>
         </is>
       </c>
     </row>
@@ -5813,7 +5813,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>0.6879438968307978</t>
+          <t>0.3138798213390375</t>
         </is>
       </c>
     </row>
@@ -5825,7 +5825,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>1.1376179486116644</t>
+          <t>3.5133361151602465</t>
         </is>
       </c>
     </row>
@@ -5873,7 +5873,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>74.34902962827766</t>
+          <t>50.03790229360589</t>
         </is>
       </c>
     </row>
@@ -5885,7 +5885,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>74.34902962827766</t>
+          <t>50.03790229360589</t>
         </is>
       </c>
     </row>
@@ -5897,7 +5897,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>74.34902962827766</t>
+          <t>50.03790229360589</t>
         </is>
       </c>
     </row>
@@ -5921,7 +5921,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>0.01480371885696002</t>
+          <t>0.03125609187307063</t>
         </is>
       </c>
     </row>
@@ -5933,7 +5933,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>0.01480371885696002</t>
+          <t>0.03125609187307063</t>
         </is>
       </c>
     </row>
@@ -5945,7 +5945,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>0.01480371885696002</t>
+          <t>0.03125609187307063</t>
         </is>
       </c>
     </row>
@@ -5957,7 +5957,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>911.5</t>
+          <t>4477.25</t>
         </is>
       </c>
     </row>
@@ -6005,7 +6005,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>551.117736220648</t>
+          <t>294.20791718180163</t>
         </is>
       </c>
     </row>
@@ -6017,7 +6017,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>551.117736220648</t>
+          <t>294.20791718180163</t>
         </is>
       </c>
     </row>
@@ -6029,7 +6029,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>551.117736220648</t>
+          <t>294.20791718180163</t>
         </is>
       </c>
     </row>
@@ -6053,7 +6053,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>5.255708214301188</t>
+          <t>3.3127204580028766</t>
         </is>
       </c>
     </row>
@@ -6065,7 +6065,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>29.13658340328295</t>
+          <t>863.4486575512709</t>
         </is>
       </c>
     </row>
@@ -6077,7 +6077,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>0.030445702528915843</t>
+          <t>0.15369217280544734</t>
         </is>
       </c>
     </row>
@@ -6089,7 +6089,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>0.05545415830139319</t>
+          <t>0.2723885137190485</t>
         </is>
       </c>
     </row>
@@ -6101,7 +6101,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>151.29026876605664</t>
+          <t>88.7270692052786</t>
         </is>
       </c>
     </row>
@@ -6113,7 +6113,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>0.03646444886926772</t>
+          <t>0.2734596874304678</t>
         </is>
       </c>
     </row>
@@ -6125,7 +6125,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>0.03646444886926772</t>
+          <t>0.2734596874304678</t>
         </is>
       </c>
     </row>
@@ -6137,7 +6137,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>0.03646444886926772</t>
+          <t>0.2734596874304678</t>
         </is>
       </c>
     </row>
@@ -6149,7 +6149,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>12.0</t>
+          <t>106.0</t>
         </is>
       </c>
     </row>
@@ -6197,7 +6197,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>2049715.0833333333</t>
+          <t>35799.688679245286</t>
         </is>
       </c>
     </row>
@@ -6209,7 +6209,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>2049715.0833333333</t>
+          <t>35799.688679245286</t>
         </is>
       </c>
     </row>
@@ -6221,7 +6221,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>2049715.0833333333</t>
+          <t>35799.688679245286</t>
         </is>
       </c>
     </row>
@@ -6245,7 +6245,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>1.0</t>
+          <t>1.528301886792453</t>
         </is>
       </c>
     </row>
@@ -6257,7 +6257,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>0.08333333333333333</t>
+          <t>0.014417942328230687</t>
         </is>
       </c>
     </row>
@@ -6269,7 +6269,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>8.018606504418755e-07</t>
+          <t>0.019687902422080288</t>
         </is>
       </c>
     </row>
@@ -6281,7 +6281,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>8.018606504418755e-07</t>
+          <t>0.019687902422080288</t>
         </is>
       </c>
     </row>
@@ -6293,7 +6293,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>8.018606504418755e-07</t>
+          <t>0.019687902422080288</t>
         </is>
       </c>
     </row>
@@ -6305,7 +6305,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>3.5849625007211516</t>
+          <t>6.260847105465749</t>
         </is>
       </c>
     </row>
@@ -6317,7 +6317,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>0.0007300602299689724</t>
+          <t>0.006448865364725923</t>
         </is>
       </c>
     </row>
@@ -6329,7 +6329,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>173500.0208333333</t>
+          <t>11754.21262014952</t>
         </is>
       </c>
     </row>
@@ -6431,7 +6431,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.5870883708257714</v>
+        <v>0.5870883708257715</v>
       </c>
     </row>
     <row r="3">
@@ -6441,7 +6441,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.1179501609873498</v>
+        <v>0.1179501609873502</v>
       </c>
     </row>
     <row r="4">
@@ -6451,7 +6451,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>12.26882798837458</v>
+        <v>12.26882798837461</v>
       </c>
     </row>
     <row r="5">
@@ -6472,7 +6472,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>90.0</t>
+          <t>64.19501538281614</t>
         </is>
       </c>
     </row>
@@ -6484,7 +6484,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>64.19501538281614</t>
+          <t>90.52071586106685</t>
         </is>
       </c>
     </row>
@@ -6496,7 +6496,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>90.52071586106685</t>
+          <t>90.0</t>
         </is>
       </c>
     </row>
@@ -6520,7 +6520,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>23495.416666666668</t>
+          <t>23576.916666666668</t>
         </is>
       </c>
     </row>
@@ -6542,7 +6542,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>0.32191335577134633</t>
+          <t>0.3227027086284717</t>
         </is>
       </c>
     </row>
@@ -6554,7 +6554,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>12323.495095080543</t>
+          <t>12321.763044272322</t>
         </is>
       </c>
     </row>
@@ -6566,7 +6566,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>0.5245063439357552</t>
+          <t>0.5226197818179076</t>
         </is>
       </c>
     </row>
@@ -6732,7 +6732,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>28.25924645039548</t>
+          <t>28.259246450395477</t>
         </is>
       </c>
     </row>
@@ -6804,7 +6804,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>82.02092533893554</t>
+          <t>81.78231654291814</t>
         </is>
       </c>
     </row>
@@ -6816,7 +6816,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>464.2482785331009</t>
+          <t>329.13983487908786</t>
         </is>
       </c>
     </row>
@@ -6828,7 +6828,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>8.79123372253927</t>
+          <t>4.8829421383276355</t>
         </is>
       </c>
     </row>
@@ -6840,7 +6840,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>12.820520985060543</t>
+          <t>10.893700373687226</t>
         </is>
       </c>
     </row>
@@ -6852,7 +6852,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>1.849757229768806</t>
+          <t>2.955136082816319</t>
         </is>
       </c>
     </row>
@@ -6864,7 +6864,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>0.7475076108066054</t>
+          <t>0.5683232899377325</t>
         </is>
       </c>
     </row>
@@ -6876,7 +6876,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>0.9923709075973743</t>
+          <t>1.2784226342795266</t>
         </is>
       </c>
     </row>
@@ -6888,7 +6888,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>1.7908663399873557</t>
+          <t>2.035933787977756</t>
         </is>
       </c>
     </row>
@@ -6900,7 +6900,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>0.8563806334045001</t>
+          <t>1.2681842586068017</t>
         </is>
       </c>
     </row>
@@ -6912,7 +6912,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>0.616801493943455</t>
+          <t>0.5589200856216024</t>
         </is>
       </c>
     </row>
@@ -6924,7 +6924,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>0.585065815200138</t>
+          <t>0.5121995782326997</t>
         </is>
       </c>
     </row>
@@ -6936,7 +6936,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>0.9937561430205955</t>
+          <t>0.9901672473612</t>
         </is>
       </c>
     </row>
@@ -6948,7 +6948,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>0.9472492215225297</t>
+          <t>0.9335101904356978</t>
         </is>
       </c>
     </row>
@@ -6960,7 +6960,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>-0.2073678239136259</t>
+          <t>-0.11803646506185317</t>
         </is>
       </c>
     </row>
@@ -6972,7 +6972,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>0.8372200619140349</t>
+          <t>0.6645998614360357</t>
         </is>
       </c>
     </row>
@@ -6984,7 +6984,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>0.4934351226128816</t>
+          <t>0.46654884606650054</t>
         </is>
       </c>
     </row>
@@ -6996,7 +6996,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>8.903831601602063</t>
+          <t>8.932930109560195</t>
         </is>
       </c>
     </row>
@@ -7008,7 +7008,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>0.03387563319849619</t>
+          <t>0.02964035254761465</t>
         </is>
       </c>
     </row>
@@ -7020,7 +7020,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>5.3313478833066625</t>
+          <t>5.521256156953849</t>
         </is>
       </c>
     </row>
@@ -7032,7 +7032,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>0.7552311442112154</t>
+          <t>0.5810208453185983</t>
         </is>
       </c>
     </row>
@@ -7044,7 +7044,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>0.06459595948501753</t>
+          <t>0.05561546315487343</t>
         </is>
       </c>
     </row>
@@ -7056,7 +7056,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>17.807663203204136</t>
+          <t>17.865860219120393</t>
         </is>
       </c>
     </row>
@@ -7068,7 +7068,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>3.8680636975191343</t>
+          <t>3.7505544294864235</t>
         </is>
       </c>
     </row>
@@ -7080,7 +7080,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>3.667569553707337</t>
+          <t>3.462209114125886</t>
         </is>
       </c>
     </row>
@@ -7092,7 +7092,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>5.621073709805425</t>
+          <t>5.3328199487154215</t>
         </is>
       </c>
     </row>
@@ -7104,7 +7104,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>4130.989755746518</t>
+          <t>5018.567624772468</t>
         </is>
       </c>
     </row>
@@ -7116,7 +7116,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>0.1748715131755712</t>
+          <t>0.2124441275355572</t>
         </is>
       </c>
     </row>
@@ -7128,7 +7128,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>2.5908792676169607</t>
+          <t>1.9031747499139091</t>
         </is>
       </c>
     </row>
@@ -7176,7 +7176,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>14.065487025356644</t>
+          <t>9.434915125089955</t>
         </is>
       </c>
     </row>
@@ -7188,7 +7188,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>1135.2299030605766</t>
+          <t>766.5860390297591</t>
         </is>
       </c>
     </row>
@@ -7200,7 +7200,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>0.20668452076460553</t>
+          <t>0.13477769550242</t>
         </is>
       </c>
     </row>
@@ -7224,7 +7224,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>0.21968244983182378</t>
+          <t>0.31289156617358377</t>
         </is>
       </c>
     </row>
@@ -7236,7 +7236,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>18.120591070259227</t>
+          <t>25.847289856120415</t>
         </is>
       </c>
     </row>
@@ -7248,7 +7248,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>0.003665291601199343</t>
+          <t>0.005180856549480977</t>
         </is>
       </c>
     </row>
@@ -7260,7 +7260,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>2274.0672722944755</t>
+          <t>2519.2851768817522</t>
         </is>
       </c>
     </row>
@@ -7272,7 +7272,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>0.13721456264587506</t>
+          <t>0.1364085778489954</t>
         </is>
       </c>
     </row>
@@ -7284,7 +7284,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>4.0925448307453</t>
+          <t>4.122034497702346</t>
         </is>
       </c>
     </row>
@@ -7296,7 +7296,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>82.83653563364774</t>
+          <t>82.648096659989</t>
         </is>
       </c>
     </row>
@@ -7308,7 +7308,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>2.737586388806821</t>
+          <t>2.1043879175831446</t>
         </is>
       </c>
     </row>
@@ -7320,7 +7320,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>222.8234908952357</t>
+          <t>172.32345237200164</t>
         </is>
       </c>
     </row>
@@ -7332,7 +7332,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>0.04081284693535755</t>
+          <t>0.031114582533886256</t>
         </is>
       </c>
     </row>
@@ -7344,7 +7344,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>0.015281343171409294</t>
+          <t>0.015306860081176921</t>
         </is>
       </c>
     </row>
@@ -7356,7 +7356,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>4.2928780999723</t>
+          <t>4.00453949988683</t>
         </is>
       </c>
     </row>
@@ -7368,7 +7368,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>9199.031285950352</t>
+          <t>12216.407308076783</t>
         </is>
       </c>
     </row>
@@ -7380,7 +7380,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>0.5535804569734117</t>
+          <t>0.6541900739721184</t>
         </is>
       </c>
     </row>
@@ -7392,7 +7392,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>0.7015726199043305</t>
+          <t>0.7819497946916141</t>
         </is>
       </c>
     </row>
@@ -7404,7 +7404,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>0.6954283218582642</t>
+          <t>0.42645213959203965</t>
         </is>
       </c>
     </row>
@@ -7416,7 +7416,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>0.7713553758905922</t>
+          <t>0.8332849364240101</t>
         </is>
       </c>
     </row>
@@ -7428,7 +7428,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>64.03741913703878</t>
+          <t>68.98875592485689</t>
         </is>
       </c>
     </row>
@@ -7440,7 +7440,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>0.01195521920356139</t>
+          <t>0.012924390447750785</t>
         </is>
       </c>
     </row>
@@ -7452,7 +7452,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>704.8059928897918</t>
+          <t>1065.8516056338028</t>
         </is>
       </c>
     </row>
@@ -7464,7 +7464,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>0.11931708022512134</t>
+          <t>0.12009595556437215</t>
         </is>
       </c>
     </row>
@@ -7476,7 +7476,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>5.291718149573567</t>
+          <t>5.207420952985519</t>
         </is>
       </c>
     </row>
@@ -7488,7 +7488,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>83.06399187404774</t>
+          <t>83.23752112676057</t>
         </is>
       </c>
     </row>
@@ -7500,7 +7500,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>93.22312510580667</t>
+          <t>19.50794366197183</t>
         </is>
       </c>
     </row>
@@ -7512,7 +7512,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>6809.5046554934825</t>
+          <t>1561.046985915493</t>
         </is>
       </c>
     </row>
@@ -7524,7 +7524,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>1.5128718931566205</t>
+          <t>0.2776125421365203</t>
         </is>
       </c>
     </row>
@@ -7536,7 +7536,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>0.016661711204767667</t>
+          <t>0.01629321570319979</t>
         </is>
       </c>
     </row>
@@ -7548,7 +7548,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>1695.126968004063</t>
+          <t>2955.1302535211266</t>
         </is>
       </c>
     </row>
@@ -7560,7 +7560,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>0.28696918368106705</t>
+          <t>0.33297242293195795</t>
         </is>
       </c>
     </row>
@@ -7572,7 +7572,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>0.5522024742621118</t>
+          <t>0.5964133455997646</t>
         </is>
       </c>
     </row>
@@ -7584,7 +7584,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>45.22637356620855</t>
+          <t>49.19127953228129</t>
         </is>
       </c>
     </row>
@@ -7596,7 +7596,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>0.009876633623061152</t>
+          <t>0.010356307620190307</t>
         </is>
       </c>
     </row>
@@ -7608,7 +7608,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>5.915623935324845</t>
+          <t>5.51061627520538</t>
         </is>
       </c>
     </row>
@@ -7620,7 +7620,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>0.2500529145324472</t>
+          <t>0.3756931803750582</t>
         </is>
       </c>
     </row>
@@ -7632,7 +7632,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>77.22989601620675</t>
+          <t>12.423049344177741</t>
         </is>
       </c>
     </row>
@@ -7644,7 +7644,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>11.846509393594468</t>
+          <t>15.161771462749808</t>
         </is>
       </c>
     </row>
@@ -7656,7 +7656,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>0.00044465309708067313</t>
+          <t>0.0003474255699209513</t>
         </is>
       </c>
     </row>
@@ -7668,7 +7668,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>94.66630168775043</t>
+          <t>125.00159906914004</t>
         </is>
       </c>
     </row>
@@ -7680,7 +7680,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>0.020627197313893</t>
+          <t>0.027331259582437945</t>
         </is>
       </c>
     </row>
@@ -7692,7 +7692,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>0.05488351407263045</t>
+          <t>0.041421181875694185</t>
         </is>
       </c>
     </row>
@@ -7744,7 +7744,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.06636270622148056</v>
+        <v>0.06636270622148019</v>
       </c>
     </row>
     <row r="4">
@@ -7754,7 +7754,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>8.029749984761613</v>
+        <v>8.029749984761569</v>
       </c>
     </row>
     <row r="5">
@@ -7764,7 +7764,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>120.9979285347847</v>
+        <v>120.9979285347846</v>
       </c>
     </row>
     <row r="6">
@@ -7775,7 +7775,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>104.00480758118829</t>
+          <t>70.00714249274856</t>
         </is>
       </c>
     </row>
@@ -7787,7 +7787,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>70.00714249274856</t>
+          <t>105.11898020814318</t>
         </is>
       </c>
     </row>
@@ -7799,7 +7799,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>105.11898020814318</t>
+          <t>104.00480758118829</t>
         </is>
       </c>
     </row>
@@ -7823,7 +7823,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>20250.5</t>
+          <t>20519.916666666668</t>
         </is>
       </c>
     </row>
@@ -7834,7 +7834,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>62.94515879244346</v>
+        <v>62.94515879244344</v>
       </c>
     </row>
     <row r="12">
@@ -7845,7 +7845,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>0.1831885841485933</t>
+          <t>0.18470999584251063</t>
         </is>
       </c>
     </row>
@@ -7857,7 +7857,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>19612.948393988787</t>
+          <t>19623.544496815608</t>
         </is>
       </c>
     </row>
@@ -7869,7 +7869,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>0.9685167474377812</t>
+          <t>0.9563169683185332</t>
         </is>
       </c>
     </row>
@@ -7891,7 +7891,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>1714.0</t>
+          <t>1798.773828125</t>
         </is>
       </c>
     </row>
@@ -7903,7 +7903,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>6172.0</t>
+          <t>4983.680175781249</t>
         </is>
       </c>
     </row>
@@ -7915,7 +7915,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>343095718506.0</t>
+          <t>246501949270.9411</t>
         </is>
       </c>
     </row>
@@ -7927,7 +7927,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>8.003248866941965</t>
+          <t>7.640876906694744</t>
         </is>
       </c>
     </row>
@@ -7939,7 +7939,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2400.0</t>
+          <t>1764.220703125</t>
         </is>
       </c>
     </row>
@@ -7951,7 +7951,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>3.254985558207785</t>
+          <t>2.957836844446989</t>
         </is>
       </c>
     </row>
@@ -7963,7 +7963,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>11553.0</t>
+          <t>8943.5361328125</t>
         </is>
       </c>
     </row>
@@ -7975,7 +7975,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>1406.8829190179065</t>
+          <t>1016.413486370395</t>
         </is>
       </c>
     </row>
@@ -7987,7 +7987,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>3730.9636777513856</t>
+          <t>3259.4342120752767</t>
         </is>
       </c>
     </row>
@@ -7999,7 +7999,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>3459.0</t>
+          <t>3126.970703125</t>
         </is>
       </c>
     </row>
@@ -8023,7 +8023,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>11553.0</t>
+          <t>8943.5361328125</t>
         </is>
       </c>
     </row>
@@ -8035,7 +8035,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>1000.152971827943</t>
+          <t>728.7578348001308</t>
         </is>
       </c>
     </row>
@@ -8047,7 +8047,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>4120.462657899295</t>
+          <t>3492.59728727941</t>
         </is>
       </c>
     </row>
@@ -8059,7 +8059,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>0.696800197940182</t>
+          <t>0.4059001796420181</t>
         </is>
       </c>
     </row>
@@ -8071,7 +8071,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>343095718506.0</t>
+          <t>246501949270.9411</t>
         </is>
       </c>
     </row>
@@ -8083,7 +8083,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>0.004692444617153417</t>
+          <t>0.005801849012549766</t>
         </is>
       </c>
     </row>
@@ -8095,7 +8095,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>3058122.550442373</t>
+          <t>1574324.428264717</t>
         </is>
       </c>
     </row>
@@ -8107,7 +8107,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>26908.49525868749</t>
+          <t>18373.29553894354</t>
         </is>
       </c>
     </row>
@@ -8119,7 +8119,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>798655640.3521831</t>
+          <t>100705310.94835672</t>
         </is>
       </c>
     </row>
@@ -8131,7 +8131,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>1324099.135520839</t>
+          <t>134549.0269677298</t>
         </is>
       </c>
     </row>
@@ -8143,7 +8143,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>15737.735354990167</t>
+          <t>5745.125838052084</t>
         </is>
       </c>
     </row>
@@ -8155,7 +8155,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>2997.670690721592</t>
+          <t>3924.7746401431727</t>
         </is>
       </c>
     </row>
@@ -8167,7 +8167,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>0.6799408836349686</t>
+          <t>0.1913228465342073</t>
         </is>
       </c>
     </row>
@@ -8179,7 +8179,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>41.66821324751565</t>
+          <t>48.64134868240853</t>
         </is>
       </c>
     </row>
@@ -8191,7 +8191,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>6.7829958563628585</t>
+          <t>6.953395178854253</t>
         </is>
       </c>
     </row>
@@ -8203,7 +8203,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>1236.8161735018928</t>
+          <t>1471.303966850348</t>
         </is>
       </c>
     </row>
@@ -8215,7 +8215,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>0.06861933086985078</t>
+          <t>0.059577293121687594</t>
         </is>
       </c>
     </row>
@@ -8227,7 +8227,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>0.027710524576336076</t>
+          <t>0.022852020066269192</t>
         </is>
       </c>
     </row>
@@ -8239,7 +8239,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>0.986731858588465</t>
+          <t>0.9721070249742207</t>
         </is>
       </c>
     </row>
@@ -8251,7 +8251,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>0.9216156734426916</t>
+          <t>0.888005944964247</t>
         </is>
       </c>
     </row>
@@ -8263,7 +8263,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>-0.21561195802724722</t>
+          <t>-0.1729093999223375</t>
         </is>
       </c>
     </row>
@@ -8275,7 +8275,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>0.9838047679711038</t>
+          <t>0.9632069991032123</t>
         </is>
       </c>
     </row>
@@ -8287,7 +8287,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>0.027589375145288333</t>
+          <t>0.023502136529601692</t>
         </is>
       </c>
     </row>
@@ -8299,7 +8299,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>154.02322085103512</t>
+          <t>133.85885086522626</t>
         </is>
       </c>
     </row>
@@ -8311,7 +8311,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>6.191042449145834e-05</t>
+          <t>7.553816661144654e-05</t>
         </is>
       </c>
     </row>
@@ -8323,7 +8323,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>14.238990620654473</t>
+          <t>13.905722241923158</t>
         </is>
       </c>
     </row>
@@ -8335,7 +8335,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>0.73034894701696</t>
+          <t>0.43908890631191266</t>
         </is>
       </c>
     </row>
@@ -8347,7 +8347,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>0.00029775480819921806</t>
+          <t>0.000311527342502993</t>
         </is>
       </c>
     </row>
@@ -8359,7 +8359,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>308.0464417020685</t>
+          <t>267.717701730452</t>
         </is>
       </c>
     </row>
@@ -8371,7 +8371,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>8.900946986473725</t>
+          <t>8.2319071428868</t>
         </is>
       </c>
     </row>
@@ -8383,7 +8383,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>4683.851511427951</t>
+          <t>2417.4751195488143</t>
         </is>
       </c>
     </row>
@@ -8395,7 +8395,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>8.335353678395913</t>
+          <t>7.875430199132992</t>
         </is>
       </c>
     </row>
@@ -8407,7 +8407,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>17714.106789390342</t>
+          <t>18572.44368566904</t>
         </is>
       </c>
     </row>
@@ -8419,7 +8419,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>0.8765888157853494</t>
+          <t>0.9190639195204395</t>
         </is>
       </c>
     </row>
@@ -8431,7 +8431,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>0.07153415249418714</t>
+          <t>0.04316964221345825</t>
         </is>
       </c>
     </row>
@@ -8443,7 +8443,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>94.82492082343626</t>
+          <t>117.2437648456057</t>
         </is>
       </c>
     </row>
@@ -8455,7 +8455,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>4892.909581670892</t>
+          <t>2518.6597323480105</t>
         </is>
       </c>
     </row>
@@ -8467,7 +8467,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>27320.254552652415</t>
+          <t>19647.585956057006</t>
         </is>
       </c>
     </row>
@@ -8479,7 +8479,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>1.2144695170229611</t>
+          <t>1.1313341250989708</t>
         </is>
       </c>
     </row>
@@ -8491,7 +8491,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>32146.309679334918</t>
+          <t>21854.233422406967</t>
         </is>
       </c>
     </row>
@@ -8503,7 +8503,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>0.003272792828672127</t>
+          <t>0.0028827908009235598</t>
         </is>
       </c>
     </row>
@@ -8515,7 +8515,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>0.0015710238401406454</t>
+          <t>0.0015837986211828426</t>
         </is>
       </c>
     </row>
@@ -8527,7 +8527,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>0.9501902436878684</t>
+          <t>0.9682111594967888</t>
         </is>
       </c>
     </row>
@@ -8539,7 +8539,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>26177.47084969099</t>
+          <t>19113.14345253805</t>
         </is>
       </c>
     </row>
@@ -8551,7 +8551,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>0.001255869132357564</t>
+          <t>0.0013141457374811977</t>
         </is>
       </c>
     </row>
@@ -8563,7 +8563,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>93.76782438639805</t>
+          <t>116.49066698212361</t>
         </is>
       </c>
     </row>
@@ -8575,7 +8575,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>0.004680550846285107</t>
+          <t>0.005795841138313658</t>
         </is>
       </c>
     </row>
@@ -8587,7 +8587,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>4902.517207818948</t>
+          <t>2521.598938059845</t>
         </is>
       </c>
     </row>
@@ -8599,7 +8599,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>27360.554039221737</t>
+          <t>19663.014326848403</t>
         </is>
       </c>
     </row>
@@ -8611,7 +8611,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>1.026311926624756</t>
+          <t>1.0164130696211242</t>
         </is>
       </c>
     </row>
@@ -8623,7 +8623,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>27955.853571000196</t>
+          <t>19938.546016669596</t>
         </is>
       </c>
     </row>
@@ -8635,7 +8635,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>0.0017361325805070643</t>
+          <t>0.0017183461996920085</t>
         </is>
       </c>
     </row>
@@ -8647,7 +8647,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>0.0015214994769496193</t>
+          <t>0.001541919606620412</t>
         </is>
       </c>
     </row>
@@ -8659,7 +8659,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>8.067556798114168</t>
+          <t>7.682704503899393</t>
         </is>
       </c>
     </row>
@@ -8671,7 +8671,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>19691.017773174688</t>
+          <t>19884.862764107173</t>
         </is>
       </c>
     </row>
@@ -8683,7 +8683,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>0.9829008817414707</t>
+          <t>0.9893341089865824</t>
         </is>
       </c>
     </row>
@@ -8695,7 +8695,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>0.9913648060174189</t>
+          <t>0.9946060965954078</t>
         </is>
       </c>
     </row>
@@ -8707,7 +8707,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>0.008809368087062633</t>
+          <t>0.005518544774245316</t>
         </is>
       </c>
     </row>
@@ -8719,7 +8719,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>0.993519174035695</t>
+          <t>0.9959661319295958</t>
         </is>
       </c>
     </row>
@@ -8731,7 +8731,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>27212.910951359176</t>
+          <t>19595.128048241266</t>
         </is>
       </c>
     </row>
@@ -8743,7 +8743,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>0.0014817290293999944</t>
+          <t>0.0015116976242283966</t>
         </is>
       </c>
     </row>
@@ -8755,7 +8755,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>90.7073495518566</t>
+          <t>114.24585355987055</t>
         </is>
       </c>
     </row>
@@ -8767,7 +8767,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>0.004645702921990094</t>
+          <t>0.005776995022242645</t>
         </is>
       </c>
     </row>
@@ -8779,7 +8779,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>4930.0624154422985</t>
+          <t>2530.7584800493687</t>
         </is>
       </c>
     </row>
@@ -8791,7 +8791,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>27477.28819462228</t>
+          <t>19710.046116504855</t>
         </is>
       </c>
     </row>
@@ -8803,7 +8803,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>1.1089372599231755</t>
+          <t>1.0666464401294498</t>
         </is>
       </c>
     </row>
@@ -8815,7 +8815,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>29940.76947503201</t>
+          <t>20826.741454288025</t>
         </is>
       </c>
     </row>
@@ -8827,7 +8827,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>0.0023496334902727727</t>
+          <t>0.002128265680566545</t>
         </is>
       </c>
     </row>
@@ -8839,7 +8839,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>0.0013667461658771584</t>
+          <t>0.001414081901195987</t>
         </is>
       </c>
     </row>
@@ -8851,7 +8851,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>18270.041638924456</t>
+          <t>18951.46875</t>
         </is>
       </c>
     </row>
@@ -8863,7 +8863,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>0.935725564093442</t>
+          <t>0.9583064699635923</t>
         </is>
       </c>
     </row>
@@ -8875,7 +8875,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>0.9748783610755442</t>
+          <t>0.9839564230492629</t>
         </is>
       </c>
     </row>
@@ -8887,7 +8887,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>26896.632238227343</t>
+          <t>19440.034116830724</t>
         </is>
       </c>
     </row>
@@ -8899,7 +8899,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>0.0012350097517870797</t>
+          <t>0.0012917809515326619</t>
         </is>
       </c>
     </row>
@@ -8911,7 +8911,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>8.214512119485223</t>
+          <t>7.785584249652091</t>
         </is>
       </c>
     </row>
@@ -8923,7 +8923,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>0.966201504354711</t>
+          <t>0.9786223277909739</t>
         </is>
       </c>
     </row>
@@ -8935,7 +8935,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>0.03775201627645046</t>
+          <t>0.02247993056210136</t>
         </is>
       </c>
     </row>
@@ -8947,7 +8947,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>0.03749026844251277</t>
+          <t>0.08756014363803473</t>
         </is>
       </c>
     </row>
@@ -8959,7 +8959,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>0.00045621281903517464</t>
+          <t>0.00028743674103002745</t>
         </is>
       </c>
     </row>
@@ -8971,7 +8971,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>1944389.280764767</t>
+          <t>1432040.2202054507</t>
         </is>
       </c>
     </row>
@@ -8983,7 +8983,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>1.5598974985021423</t>
+          <t>1.8315213024437824</t>
         </is>
       </c>
     </row>
@@ -8995,7 +8995,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>34.65100230304412</t>
+          <t>10.181439206275076</t>
         </is>
       </c>
     </row>

</xml_diff>